<commit_message>
Test NA e TC 24
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sviluppo\github\ministero-salute\it-fse-accreditamento\GATEWAY\A1#111GRUPPOGPI00\ARKO_SRL\cartella_emofilia_rer\1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3801DA1B-440E-4593-84FA-D7BF4CED2D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E15425-5E12-4415-838D-177491DA0990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="447">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1728,6 +1728,18 @@
   </si>
   <si>
     <t>Correggere anagrafica paziente</t>
+  </si>
+  <si>
+    <t>Se è assente la diagnosi del paziente, il quesito diagnostico viene omesso in toto</t>
+  </si>
+  <si>
+    <t>76fe52d2ec57f95d</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.7755b73f171852c</t>
+  </si>
+  <si>
+    <t>12:45:08.007</t>
   </si>
 </sst>
 </file>
@@ -3792,10 +3804,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="Q23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B131" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="V117" sqref="V117"/>
+      <selection pane="bottomRight" activeCell="J170" sqref="J170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4267,7 +4279,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
         <v>32</v>
       </c>
@@ -4563,7 +4575,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
         <v>40</v>
       </c>
@@ -4867,7 +4879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31">
         <v>48</v>
       </c>
@@ -8118,7 +8130,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A118" s="31">
         <v>154</v>
       </c>
@@ -8138,8 +8150,12 @@
       <c r="G118" s="33"/>
       <c r="H118" s="33"/>
       <c r="I118" s="39"/>
-      <c r="J118" s="29"/>
-      <c r="K118" s="29"/>
+      <c r="J118" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K118" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L118" s="29"/>
       <c r="M118" s="29"/>
       <c r="N118" s="29"/>
@@ -8155,7 +8171,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A119" s="31">
         <v>155</v>
       </c>
@@ -8175,8 +8191,12 @@
       <c r="G119" s="33"/>
       <c r="H119" s="33"/>
       <c r="I119" s="39"/>
-      <c r="J119" s="29"/>
-      <c r="K119" s="29"/>
+      <c r="J119" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K119" s="29" t="s">
+        <v>240</v>
+      </c>
       <c r="L119" s="29"/>
       <c r="M119" s="29"/>
       <c r="N119" s="29"/>
@@ -8192,7 +8212,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A120" s="31">
         <v>156</v>
       </c>
@@ -8212,8 +8232,12 @@
       <c r="G120" s="33"/>
       <c r="H120" s="33"/>
       <c r="I120" s="39"/>
-      <c r="J120" s="29"/>
-      <c r="K120" s="29"/>
+      <c r="J120" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K120" s="29" t="s">
+        <v>243</v>
+      </c>
       <c r="L120" s="29"/>
       <c r="M120" s="29"/>
       <c r="N120" s="29"/>
@@ -8229,7 +8253,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A121" s="31">
         <v>158</v>
       </c>
@@ -8249,8 +8273,12 @@
       <c r="G121" s="33"/>
       <c r="H121" s="33"/>
       <c r="I121" s="39"/>
-      <c r="J121" s="29"/>
-      <c r="K121" s="29"/>
+      <c r="J121" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K121" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L121" s="29"/>
       <c r="M121" s="29"/>
       <c r="N121" s="29"/>
@@ -8266,7 +8294,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A122" s="31">
         <v>159</v>
       </c>
@@ -8286,8 +8314,12 @@
       <c r="G122" s="33"/>
       <c r="H122" s="33"/>
       <c r="I122" s="39"/>
-      <c r="J122" s="29"/>
-      <c r="K122" s="29"/>
+      <c r="J122" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K122" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L122" s="29"/>
       <c r="M122" s="29"/>
       <c r="N122" s="29"/>
@@ -8303,7 +8335,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A123" s="31">
         <v>160</v>
       </c>
@@ -8323,8 +8355,12 @@
       <c r="G123" s="33"/>
       <c r="H123" s="33"/>
       <c r="I123" s="39"/>
-      <c r="J123" s="29"/>
-      <c r="K123" s="29"/>
+      <c r="J123" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K123" s="29" t="s">
+        <v>241</v>
+      </c>
       <c r="L123" s="29"/>
       <c r="M123" s="29"/>
       <c r="N123" s="29"/>
@@ -8340,7 +8376,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A124" s="31">
         <v>161</v>
       </c>
@@ -8360,8 +8396,12 @@
       <c r="G124" s="33"/>
       <c r="H124" s="33"/>
       <c r="I124" s="39"/>
-      <c r="J124" s="29"/>
-      <c r="K124" s="29"/>
+      <c r="J124" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K124" s="29" t="s">
+        <v>240</v>
+      </c>
       <c r="L124" s="29"/>
       <c r="M124" s="29"/>
       <c r="N124" s="29"/>
@@ -8377,7 +8417,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="31">
         <v>162</v>
       </c>
@@ -8397,9 +8437,15 @@
       <c r="G125" s="33"/>
       <c r="H125" s="33"/>
       <c r="I125" s="39"/>
-      <c r="J125" s="29"/>
-      <c r="K125" s="29"/>
-      <c r="L125" s="29"/>
+      <c r="J125" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K125" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="L125" s="29" t="s">
+        <v>443</v>
+      </c>
       <c r="M125" s="29"/>
       <c r="N125" s="29"/>
       <c r="O125" s="29"/>
@@ -8414,7 +8460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="31">
         <v>163</v>
       </c>
@@ -8434,8 +8480,12 @@
       <c r="G126" s="33"/>
       <c r="H126" s="33"/>
       <c r="I126" s="39"/>
-      <c r="J126" s="29"/>
-      <c r="K126" s="29"/>
+      <c r="J126" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K126" s="29" t="s">
+        <v>241</v>
+      </c>
       <c r="L126" s="29"/>
       <c r="M126" s="29"/>
       <c r="N126" s="29"/>
@@ -8451,7 +8501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="31">
         <v>164</v>
       </c>
@@ -8471,8 +8521,12 @@
       <c r="G127" s="33"/>
       <c r="H127" s="33"/>
       <c r="I127" s="39"/>
-      <c r="J127" s="29"/>
-      <c r="K127" s="29"/>
+      <c r="J127" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K127" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L127" s="29"/>
       <c r="M127" s="29"/>
       <c r="N127" s="29"/>
@@ -8488,7 +8542,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="31">
         <v>165</v>
       </c>
@@ -8508,8 +8562,12 @@
       <c r="G128" s="33"/>
       <c r="H128" s="33"/>
       <c r="I128" s="39"/>
-      <c r="J128" s="29"/>
-      <c r="K128" s="29"/>
+      <c r="J128" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K128" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L128" s="29"/>
       <c r="M128" s="29"/>
       <c r="N128" s="29"/>
@@ -8525,7 +8583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A129" s="31">
         <v>166</v>
       </c>
@@ -8545,8 +8603,12 @@
       <c r="G129" s="33"/>
       <c r="H129" s="33"/>
       <c r="I129" s="39"/>
-      <c r="J129" s="29"/>
-      <c r="K129" s="29"/>
+      <c r="J129" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K129" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L129" s="29"/>
       <c r="M129" s="29"/>
       <c r="N129" s="29"/>
@@ -8562,7 +8624,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A130" s="31">
         <v>167</v>
       </c>
@@ -8582,8 +8644,12 @@
       <c r="G130" s="33"/>
       <c r="H130" s="33"/>
       <c r="I130" s="39"/>
-      <c r="J130" s="29"/>
-      <c r="K130" s="29"/>
+      <c r="J130" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K130" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L130" s="29"/>
       <c r="M130" s="29"/>
       <c r="N130" s="29"/>
@@ -8599,7 +8665,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A131" s="31">
         <v>168</v>
       </c>
@@ -8619,8 +8685,12 @@
       <c r="G131" s="33"/>
       <c r="H131" s="33"/>
       <c r="I131" s="39"/>
-      <c r="J131" s="29"/>
-      <c r="K131" s="29"/>
+      <c r="J131" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K131" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L131" s="29"/>
       <c r="M131" s="29"/>
       <c r="N131" s="29"/>
@@ -8636,7 +8706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:23" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="31">
         <v>169</v>
       </c>
@@ -8656,8 +8726,12 @@
       <c r="G132" s="33"/>
       <c r="H132" s="33"/>
       <c r="I132" s="39"/>
-      <c r="J132" s="29"/>
-      <c r="K132" s="29"/>
+      <c r="J132" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K132" s="29" t="s">
+        <v>241</v>
+      </c>
       <c r="L132" s="29"/>
       <c r="M132" s="29"/>
       <c r="N132" s="29"/>
@@ -10005,7 +10079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:23" ht="115.8" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A169" s="31">
         <v>447</v>
       </c>
@@ -10042,7 +10116,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="170" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:23" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A170" s="31">
         <v>448</v>
       </c>
@@ -10058,11 +10132,21 @@
       <c r="E170" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="F170" s="33"/>
-      <c r="G170" s="33"/>
-      <c r="H170" s="33"/>
-      <c r="I170" s="39"/>
-      <c r="J170" s="29"/>
+      <c r="F170" s="33">
+        <v>45755</v>
+      </c>
+      <c r="G170" s="33" t="s">
+        <v>446</v>
+      </c>
+      <c r="H170" s="33" t="s">
+        <v>444</v>
+      </c>
+      <c r="I170" s="39" t="s">
+        <v>445</v>
+      </c>
+      <c r="J170" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="K170" s="29"/>
       <c r="L170" s="29"/>
       <c r="M170" s="29"/>
@@ -17263,27 +17347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17541,32 +17604,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17583,4 +17642,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Mancano solo test per JWT token
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sviluppo\github\ministero-salute\it-fse-accreditamento\GATEWAY\A1#111GRUPPOGPI00\ARKO_SRL\cartella_emofilia_rer\1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E15425-5E12-4415-838D-177491DA0990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8F857E-9B72-4209-A84E-E7D18A31495F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="447">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -3804,10 +3804,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B131" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J170" sqref="J170"/>
+      <selection pane="bottomRight" activeCell="L189" sqref="L189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10163,7 +10163,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="171" spans="1:23" ht="10.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:23" ht="129" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A171" s="31">
         <v>449</v>
       </c>
@@ -10183,8 +10183,12 @@
       <c r="G171" s="33"/>
       <c r="H171" s="33"/>
       <c r="I171" s="39"/>
-      <c r="J171" s="29"/>
-      <c r="K171" s="29"/>
+      <c r="J171" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K171" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L171" s="29"/>
       <c r="M171" s="29"/>
       <c r="N171" s="29"/>
@@ -10533,7 +10537,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="181" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:23" ht="14.4" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A181" s="31">
         <v>460</v>
       </c>
@@ -10570,7 +10574,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:23" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A182" s="31">
         <v>461</v>
       </c>
@@ -10583,15 +10587,19 @@
       <c r="D182" s="31" t="s">
         <v>402</v>
       </c>
-      <c r="E182" s="31" t="s">
+      <c r="E182" s="32" t="s">
         <v>401</v>
       </c>
       <c r="F182" s="31"/>
       <c r="G182" s="31"/>
       <c r="H182" s="31"/>
       <c r="I182" s="31"/>
-      <c r="J182" s="31"/>
-      <c r="K182" s="31"/>
+      <c r="J182" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K182" s="29" t="s">
+        <v>239</v>
+      </c>
       <c r="L182" s="31"/>
       <c r="M182" s="31"/>
       <c r="N182" s="31"/>
@@ -10792,7 +10800,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="188" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:23" ht="3.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A188" s="31">
         <v>467</v>
       </c>
@@ -10829,7 +10837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="189" spans="1:23" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:23" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A189" s="31">
         <v>468</v>
       </c>
@@ -10849,8 +10857,12 @@
       <c r="G189" s="31"/>
       <c r="H189" s="31"/>
       <c r="I189" s="31"/>
-      <c r="J189" s="31"/>
-      <c r="K189" s="31"/>
+      <c r="J189" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="K189" s="29" t="s">
+        <v>241</v>
+      </c>
       <c r="L189" s="31"/>
       <c r="M189" s="31"/>
       <c r="N189" s="31"/>
@@ -10866,7 +10878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="190" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:23" ht="73.8" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A190" s="31">
         <v>469</v>
       </c>
@@ -10903,7 +10915,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="191" spans="1:23" ht="14.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:23" ht="115.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A191" s="31">
         <v>470</v>
       </c>
@@ -15084,7 +15096,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 M14:N14 P14:R14 J16:J20 M16:N20 P16:R20 J22 M22:N22 P22:R22 J24:J28 M24:N28 P24:R28 P10:R12 M10:N12 J10:J12 P30:R180 J30:J180 M30:N180</xm:sqref>
+          <xm:sqref>J14 M14:N14 P14:R14 J16:J20 M16:N20 P16:R20 J22 M22:N22 P22:R22 J24:J28 M24:N28 P24:R28 P10:R12 M10:N12 J10:J12 P30:R180 J30:J180 M30:N180 J182 J189</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -15096,7 +15108,7 @@
           <x14:formula1>
             <xm:f>'LISTA VALORI'!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>K10:K180</xm:sqref>
+          <xm:sqref>K10:K180 K182 K189</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -17347,6 +17359,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17604,28 +17637,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17642,29 +17679,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Completati i test case
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
+++ b/GATEWAY/A1#111GRUPPOGPI00/ARKO_SRL/cartella_emofilia_rer/1.2/cartella-emofilia-rer-accreditamento-checklist_V8.2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sviluppo\github\ministero-salute\it-fse-accreditamento\GATEWAY\A1#111GRUPPOGPI00\ARKO_SRL\cartella_emofilia_rer\1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8F857E-9B72-4209-A84E-E7D18A31495F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993F7ED4-9559-4DE1-9842-3DDC9E03DE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="463">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1740,6 +1740,54 @@
   </si>
   <si>
     <t>12:45:08.007</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>14:42:47.150</t>
+  </si>
+  <si>
+    <t>Il campo purpose_of_use non ???? valorizzato</t>
+  </si>
+  <si>
+    <t>f38575cab2a25c6d</t>
+  </si>
+  <si>
+    <t>14:48:51.593</t>
+  </si>
+  <si>
+    <t>Il campo action_id non ???? corretto</t>
+  </si>
+  <si>
+    <t>14:52:31.223</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> il programma memorizza nel DB il messaggio di errore che proviene dal servizio di validazione per analisi successiva in backoffice. Una volta corretta la configurazione dell'integrazione (in questo caso il parametro purpose_of_use)  l'utente dovrà rigenerare il referto e firmarlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> il programma memorizza nel DB il messaggio di errore che proviene dal servizio di validazione per analisi successiva in backoffice. Una volta corretta la configurazione dell'integrazione (in questo caso il parametro action_id)  l'utente dovrà rigenerare il referto e firmarlo</t>
+  </si>
+  <si>
+    <t>Impossibile raggiungere il gateway di validazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eventuali re-invii di validazione vengono concordati/definiti con le singole Aziende. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viene messo a disposizione dell'Azienda una modalità di verifica dei documenti che hanno avuto errori di validazione </t>
+  </si>
+  <si>
+    <t>da parte del gateway per poterli individuare e procedere alla correzione, firma e re-invio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gli utenti abilitati (ad esempio le figure di Back-office concordate con l'Azienda) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">possono accedere ai dati e consultare eventuali errori andando ad individuare i referti da correggere. </t>
+  </si>
+  <si>
+    <t>Il processo di firma viene bloccato. Una volta risolto il problema che scatena il timeout,  l'utente dovrà rigenerare il referto e firmarlo</t>
   </si>
 </sst>
 </file>
@@ -3804,10 +3852,10 @@
   <dimension ref="A1:W756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B171" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="N31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L189" sqref="L189"/>
+      <selection pane="bottomRight" activeCell="S117" sqref="S117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4279,7 +4327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="173.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31">
         <v>32</v>
       </c>
@@ -4295,20 +4343,44 @@
       <c r="E15" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="29"/>
+      <c r="F15" s="33">
+        <v>45755</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>448</v>
+      </c>
+      <c r="H15" s="33">
+        <v>7599619418747600</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="J15" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="29"/>
-      <c r="R15" s="29"/>
-      <c r="S15" s="29"/>
+      <c r="M15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="O15" s="29" t="s">
+        <v>449</v>
+      </c>
+      <c r="P15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q15" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="R15" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S15" s="29" t="s">
+        <v>454</v>
+      </c>
       <c r="T15" s="29"/>
       <c r="U15" s="34"/>
       <c r="V15" s="35"/>
@@ -4538,7 +4610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" ht="1.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="31">
         <v>39</v>
       </c>
@@ -4575,7 +4647,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="20.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31">
         <v>40</v>
       </c>
@@ -4591,20 +4663,44 @@
       <c r="E23" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="29"/>
+      <c r="F23" s="33">
+        <v>45755</v>
+      </c>
+      <c r="G23" s="33" t="s">
+        <v>451</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>450</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="K23" s="29"/>
       <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="29"/>
-      <c r="Q23" s="29"/>
-      <c r="R23" s="29"/>
-      <c r="S23" s="29"/>
+      <c r="M23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="O23" s="29" t="s">
+        <v>452</v>
+      </c>
+      <c r="P23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="R23" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S23" s="29" t="s">
+        <v>455</v>
+      </c>
       <c r="T23" s="29"/>
       <c r="U23" s="34"/>
       <c r="V23" s="35"/>
@@ -4840,7 +4936,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="10.95" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:23" ht="88.2" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="31">
         <v>47</v>
       </c>
@@ -4879,7 +4975,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:23" ht="116.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="31">
         <v>48</v>
       </c>
@@ -4895,20 +4991,36 @@
       <c r="E31" s="32" t="s">
         <v>246</v>
       </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
+      <c r="F31" s="33">
+        <v>45755</v>
+      </c>
+      <c r="G31" s="33" t="s">
+        <v>453</v>
+      </c>
       <c r="H31" s="33"/>
       <c r="I31" s="39"/>
       <c r="J31" s="29"/>
       <c r="K31" s="29"/>
       <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
-      <c r="O31" s="29"/>
-      <c r="P31" s="29"/>
+      <c r="M31" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="N31" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="P31" s="29" t="s">
+        <v>66</v>
+      </c>
       <c r="Q31" s="29"/>
-      <c r="R31" s="29"/>
-      <c r="S31" s="29"/>
+      <c r="R31" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="S31" s="29" t="s">
+        <v>462</v>
+      </c>
       <c r="T31" s="29"/>
       <c r="U31" s="34" t="s">
         <v>66</v>
@@ -4947,7 +5059,9 @@
       <c r="P32" s="29"/>
       <c r="Q32" s="29"/>
       <c r="R32" s="29"/>
-      <c r="S32" s="29"/>
+      <c r="S32" s="29" t="s">
+        <v>457</v>
+      </c>
       <c r="T32" s="29"/>
       <c r="U32" s="34" t="s">
         <v>66</v>
@@ -4986,7 +5100,9 @@
       <c r="P33" s="29"/>
       <c r="Q33" s="29"/>
       <c r="R33" s="29"/>
-      <c r="S33" s="29"/>
+      <c r="S33" s="29" t="s">
+        <v>458</v>
+      </c>
       <c r="T33" s="29"/>
       <c r="U33" s="34" t="s">
         <v>66</v>
@@ -5025,7 +5141,9 @@
       <c r="P34" s="29"/>
       <c r="Q34" s="29"/>
       <c r="R34" s="29"/>
-      <c r="S34" s="29"/>
+      <c r="S34" s="29" t="s">
+        <v>459</v>
+      </c>
       <c r="T34" s="29"/>
       <c r="U34" s="34" t="s">
         <v>66</v>
@@ -5064,7 +5182,9 @@
       <c r="P35" s="29"/>
       <c r="Q35" s="29"/>
       <c r="R35" s="29"/>
-      <c r="S35" s="29"/>
+      <c r="S35" s="29" t="s">
+        <v>460</v>
+      </c>
       <c r="T35" s="29"/>
       <c r="U35" s="34"/>
       <c r="V35" s="35"/>
@@ -5101,7 +5221,9 @@
       <c r="P36" s="29"/>
       <c r="Q36" s="29"/>
       <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
+      <c r="S36" s="29" t="s">
+        <v>461</v>
+      </c>
       <c r="T36" s="29"/>
       <c r="U36" s="34"/>
       <c r="V36" s="35"/>
@@ -15096,7 +15218,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14 M14:N14 P14:R14 J16:J20 M16:N20 P16:R20 J22 M22:N22 P22:R22 J24:J28 M24:N28 P24:R28 P10:R12 M10:N12 J10:J12 P30:R180 J30:J180 M30:N180 J182 J189</xm:sqref>
+          <xm:sqref>J14 M14:N14 P14:R14 J16:J20 M16:N20 P16:R20 J22 M22:N22 P22:R22 J24:J28 M24:N28 P24:R28 P10:R12 M10:N12 J10:J12 P30:R180 J30:J180 J189 J182 M30:N30 M32:N180</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{70793024-27E9-4E6A-BACD-083AB683BC38}">
           <x14:formula1>
@@ -17359,27 +17481,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17637,32 +17738,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CE213DB-5082-48B0-B2A5-099EBF944035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17679,4 +17776,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>